<commit_message>
Switches: - rename a file - add a standoff - PCB layout tweaks
</commit_message>
<xml_diff>
--- a/modules/Switches/Switches-BOM.xlsx
+++ b/modules/Switches/Switches-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Switches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36ADEE1-2D76-43A5-A127-6E8F208E6D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75746D3E-6443-472E-B825-39FE5370466B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="1110" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7080" yWindow="690" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches-BOM" sheetId="1" r:id="rId1"/>
@@ -203,18 +203,12 @@
     <t>https://www.mouser.ca/ProductDetail/810-FG18X7R1H102KNT6</t>
   </si>
   <si>
-    <t>H1 H5</t>
-  </si>
-  <si>
     <t>HW_Screw_M3x0.50x6</t>
   </si>
   <si>
     <t>Machine screw, M3x0.50x6</t>
   </si>
   <si>
-    <t>H3</t>
-  </si>
-  <si>
     <t>HW_Standoff_F-F_11mm_M3x0.50</t>
   </si>
   <si>
@@ -591,6 +585,12 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>H1 H5 H6 H10</t>
+  </si>
+  <si>
+    <t>H3 H8</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1446,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,13 +1463,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1699,85 +1699,85 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
         <v>57</v>
-      </c>
-      <c r="I6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>185</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
         <v>60</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>61</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>62</v>
-      </c>
-      <c r="K7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" t="s">
-        <v>64</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P7" t="s">
         <v>35</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S7" t="s">
         <v>35</v>
       </c>
       <c r="T7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1790,16 +1790,16 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" t="s">
         <v>72</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>73</v>
-      </c>
-      <c r="J8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" t="s">
-        <v>75</v>
       </c>
       <c r="L8">
         <v>61201621621</v>
@@ -1808,15 +1808,15 @@
         <v>35</v>
       </c>
       <c r="N8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1829,51 +1829,51 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" t="s">
         <v>79</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>80</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>81</v>
-      </c>
-      <c r="K9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" t="s">
-        <v>83</v>
       </c>
       <c r="M9" t="s">
         <v>22</v>
       </c>
       <c r="N9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
       </c>
       <c r="Q9" t="s">
+        <v>84</v>
+      </c>
+      <c r="R9" t="s">
+        <v>85</v>
+      </c>
+      <c r="S9" t="s">
         <v>86</v>
-      </c>
-      <c r="R9" t="s">
-        <v>87</v>
-      </c>
-      <c r="S9" t="s">
-        <v>88</v>
       </c>
       <c r="T9">
         <v>4031</v>
       </c>
       <c r="U9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1886,36 +1886,36 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" t="s">
         <v>91</v>
       </c>
-      <c r="I10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" t="s">
-        <v>93</v>
-      </c>
       <c r="M10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N10">
         <v>598</v>
       </c>
       <c r="O10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P10" t="s">
         <v>35</v>
       </c>
       <c r="Q10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1928,36 +1928,36 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N11">
         <v>598</v>
       </c>
       <c r="O11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P11" t="s">
         <v>35</v>
       </c>
       <c r="Q11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1970,33 +1970,33 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N12">
         <v>392</v>
       </c>
       <c r="O12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P12" t="s">
         <v>35</v>
       </c>
       <c r="Q12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2009,33 +2009,33 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N13">
         <v>392</v>
       </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P13" t="s">
         <v>35</v>
       </c>
       <c r="Q13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2048,33 +2048,33 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" t="s">
         <v>107</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>108</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>109</v>
-      </c>
-      <c r="K14" t="s">
-        <v>110</v>
-      </c>
-      <c r="L14" t="s">
-        <v>111</v>
       </c>
       <c r="M14" t="s">
         <v>35</v>
       </c>
       <c r="N14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -2087,33 +2087,33 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" t="s">
         <v>115</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>116</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>117</v>
-      </c>
-      <c r="K15" t="s">
-        <v>118</v>
-      </c>
-      <c r="L15" t="s">
-        <v>119</v>
       </c>
       <c r="M15" t="s">
         <v>35</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -2129,36 +2129,36 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" t="s">
         <v>123</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>124</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>125</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>126</v>
-      </c>
-      <c r="K16" t="s">
-        <v>127</v>
-      </c>
-      <c r="L16" t="s">
-        <v>128</v>
       </c>
       <c r="M16" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -2171,36 +2171,36 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" t="s">
+        <v>123</v>
+      </c>
+      <c r="J17" t="s">
         <v>124</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>125</v>
       </c>
-      <c r="J17" t="s">
-        <v>126</v>
-      </c>
-      <c r="K17" t="s">
-        <v>127</v>
-      </c>
       <c r="L17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M17" t="s">
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2213,39 +2213,39 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" t="s">
         <v>138</v>
       </c>
-      <c r="H18" t="s">
+      <c r="K18" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" t="s">
         <v>139</v>
-      </c>
-      <c r="I18" t="s">
-        <v>125</v>
-      </c>
-      <c r="J18" t="s">
-        <v>140</v>
-      </c>
-      <c r="K18" t="s">
-        <v>127</v>
-      </c>
-      <c r="L18" t="s">
-        <v>141</v>
       </c>
       <c r="M18" t="s">
         <v>35</v>
       </c>
       <c r="N18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2258,36 +2258,36 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" t="s">
         <v>124</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>125</v>
       </c>
-      <c r="J19" t="s">
-        <v>126</v>
-      </c>
-      <c r="K19" t="s">
-        <v>127</v>
-      </c>
       <c r="L19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M19" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2300,39 +2300,39 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" t="s">
         <v>124</v>
       </c>
-      <c r="H20" t="s">
-        <v>139</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>125</v>
       </c>
-      <c r="J20" t="s">
-        <v>126</v>
-      </c>
-      <c r="K20" t="s">
-        <v>127</v>
-      </c>
       <c r="L20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2345,39 +2345,39 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" t="s">
         <v>138</v>
       </c>
-      <c r="H21" t="s">
+      <c r="K21" t="s">
+        <v>154</v>
+      </c>
+      <c r="L21" t="s">
         <v>155</v>
-      </c>
-      <c r="I21" t="s">
-        <v>125</v>
-      </c>
-      <c r="J21" t="s">
-        <v>140</v>
-      </c>
-      <c r="K21" t="s">
-        <v>156</v>
-      </c>
-      <c r="L21" t="s">
-        <v>157</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -2393,33 +2393,33 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" t="s">
         <v>161</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>162</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>163</v>
-      </c>
-      <c r="K22" t="s">
-        <v>164</v>
-      </c>
-      <c r="L22" t="s">
-        <v>165</v>
       </c>
       <c r="M22" t="s">
         <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="O22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2432,33 +2432,33 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
+        <v>167</v>
+      </c>
+      <c r="I23" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" t="s">
         <v>169</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>170</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>171</v>
-      </c>
-      <c r="K23" t="s">
-        <v>172</v>
-      </c>
-      <c r="L23" t="s">
-        <v>173</v>
       </c>
       <c r="M23" t="s">
         <v>35</v>
       </c>
       <c r="N23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="O23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2471,28 +2471,28 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="I24" t="s">
+        <v>176</v>
+      </c>
+      <c r="J24" t="s">
         <v>177</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" t="s">
         <v>178</v>
-      </c>
-      <c r="J24" t="s">
-        <v>179</v>
-      </c>
-      <c r="K24" t="s">
-        <v>172</v>
-      </c>
-      <c r="L24" t="s">
-        <v>180</v>
       </c>
       <c r="M24" t="s">
         <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="O24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switches - BOM update
</commit_message>
<xml_diff>
--- a/modules/Switches/Switches-BOM.xlsx
+++ b/modules/Switches/Switches-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Switches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75746D3E-6443-472E-B825-39FE5370466B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05E0743-DBE1-4789-8434-6307052DE718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="690" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="840" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches-BOM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="185">
   <si>
     <t>Ref</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>5%, 1/4 W</t>
-  </si>
-  <si>
-    <t>as req'd</t>
   </si>
   <si>
     <t>https://www.mouser.ca/datasheet/2/427/ccf07-1762725.pdf</t>
@@ -1446,7 +1443,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,13 +1460,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1665,8 +1662,8 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>10</v>
+      <c r="C5">
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -1699,7 +1696,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1720,7 +1717,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2079,7 +2076,7 @@
       <c r="B15">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="C15">
         <v>12</v>
       </c>
       <c r="E15">
@@ -2119,10 +2116,7 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -2205,8 +2199,8 @@
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="D18">
-        <v>10</v>
+      <c r="C18">
+        <v>4</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -2218,34 +2212,31 @@
       <c r="G18" t="s">
         <v>136</v>
       </c>
-      <c r="H18" t="s">
-        <v>137</v>
-      </c>
       <c r="I18" t="s">
         <v>123</v>
       </c>
       <c r="J18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K18" t="s">
         <v>125</v>
       </c>
       <c r="L18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M18" t="s">
         <v>35</v>
       </c>
       <c r="N18" t="s">
+        <v>139</v>
+      </c>
+      <c r="O18" t="s">
         <v>140</v>
-      </c>
-      <c r="O18" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2258,7 +2249,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G19" t="s">
         <v>122</v>
@@ -2273,21 +2264,21 @@
         <v>125</v>
       </c>
       <c r="L19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M19" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19" t="s">
         <v>145</v>
-      </c>
-      <c r="O19" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2300,14 +2291,11 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G20" t="s">
         <v>122</v>
       </c>
-      <c r="H20" t="s">
-        <v>137</v>
-      </c>
       <c r="I20" t="s">
         <v>123</v>
       </c>
@@ -2318,21 +2306,21 @@
         <v>125</v>
       </c>
       <c r="L20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" t="s">
         <v>150</v>
-      </c>
-      <c r="O20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2351,41 +2339,38 @@
         <v>136</v>
       </c>
       <c r="H21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I21" t="s">
         <v>123</v>
       </c>
       <c r="J21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K21" t="s">
+        <v>153</v>
+      </c>
+      <c r="L21" t="s">
         <v>154</v>
-      </c>
-      <c r="L21" t="s">
-        <v>155</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
+        <v>155</v>
+      </c>
+      <c r="O21" t="s">
         <v>156</v>
-      </c>
-      <c r="O21" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
       <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
         <v>4</v>
       </c>
       <c r="E22">
@@ -2393,33 +2378,33 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" t="s">
         <v>159</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>160</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>161</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>162</v>
-      </c>
-      <c r="L22" t="s">
-        <v>163</v>
       </c>
       <c r="M22" t="s">
         <v>35</v>
       </c>
       <c r="N22" t="s">
+        <v>163</v>
+      </c>
+      <c r="O22" t="s">
         <v>164</v>
-      </c>
-      <c r="O22" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2432,33 +2417,33 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
+        <v>166</v>
+      </c>
+      <c r="I23" t="s">
         <v>167</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>168</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>169</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>170</v>
-      </c>
-      <c r="L23" t="s">
-        <v>171</v>
       </c>
       <c r="M23" t="s">
         <v>35</v>
       </c>
       <c r="N23" t="s">
+        <v>171</v>
+      </c>
+      <c r="O23" t="s">
         <v>172</v>
-      </c>
-      <c r="O23" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2471,28 +2456,28 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
+        <v>174</v>
+      </c>
+      <c r="I24" t="s">
         <v>175</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>176</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
+        <v>169</v>
+      </c>
+      <c r="L24" t="s">
         <v>177</v>
-      </c>
-      <c r="K24" t="s">
-        <v>170</v>
-      </c>
-      <c r="L24" t="s">
-        <v>178</v>
       </c>
       <c r="M24" t="s">
         <v>35</v>
       </c>
       <c r="N24" t="s">
+        <v>178</v>
+      </c>
+      <c r="O24" t="s">
         <v>179</v>
-      </c>
-      <c r="O24" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>